<commit_message>
repair table of decisions and general code
</commit_message>
<xml_diff>
--- a/tabela decyzyjna.xlsx
+++ b/tabela decyzyjna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub Korban\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakubkorban/Documents/GitHub/Loty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B6A68C-6481-4CA0-94FA-A8C28407CD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD027CE6-1663-8442-955F-B39A90736871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13455" yWindow="45" windowWidth="15195" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="27">
   <si>
     <t>Czy krajowy?</t>
   </si>
@@ -71,29 +71,56 @@
     <t>WYNIK: Jaka zniżka? (%)</t>
   </si>
   <si>
-    <t>Dzieci &lt; 2</t>
-  </si>
-  <si>
     <t>Dorośli</t>
   </si>
   <si>
-    <t xml:space="preserve">Młodzież &lt;2; 16&gt; </t>
-  </si>
-  <si>
-    <t>MAX 80</t>
-  </si>
-  <si>
     <t>MAX 30</t>
   </si>
   <si>
     <t>MAX  30</t>
+  </si>
+  <si>
+    <t>Młodzież &lt;17; 18)</t>
+  </si>
+  <si>
+    <t>Dzieci &lt; 0; 2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Młodzież (2; 17) </t>
+  </si>
+  <si>
+    <t>15% gdy T</t>
+  </si>
+  <si>
+    <t>10% Dla T</t>
+  </si>
+  <si>
+    <t>80% Dla T</t>
+  </si>
+  <si>
+    <t>70% Dla T</t>
+  </si>
+  <si>
+    <t>15% gdy T dla M</t>
+  </si>
+  <si>
+    <t>MAX 80, 70 dla M</t>
+  </si>
+  <si>
+    <t>"+"</t>
+  </si>
+  <si>
+    <t>15% gdy T , gdy N 0%</t>
+  </si>
+  <si>
+    <t>15% gdy T, gdy N 0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +154,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +205,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -199,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,9 +260,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -238,6 +281,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,32 +587,36 @@
   <dimension ref="A1:KN258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B50" sqref="B50:E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="29.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="2" customWidth="1"/>
+    <col min="3" max="9" width="9.1640625" style="2"/>
+    <col min="10" max="10" width="18.5" style="2" customWidth="1"/>
+    <col min="11" max="17" width="9.1640625" style="2"/>
+    <col min="18" max="18" width="25.6640625" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1</v>
@@ -575,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -603,8 +671,11 @@
       <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -632,66 +703,69 @@
       <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -719,8 +793,11 @@
       <c r="I9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -748,37 +825,40 @@
       <c r="I10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -807,17 +887,41 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>1</v>
@@ -844,11 +948,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -860,20 +964,23 @@
       <c r="E18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -889,78 +996,81 @@
       <c r="E19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -976,20 +1086,23 @@
       <c r="E22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1005,88 +1118,115 @@
       <c r="E23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="3">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3">
+        <v>10</v>
+      </c>
+      <c r="F25" s="14">
         <v>30</v>
       </c>
-      <c r="C25" s="3">
+      <c r="G25" s="14">
         <v>0</v>
       </c>
-      <c r="D25" s="3">
+      <c r="H25" s="14">
         <v>25</v>
       </c>
-      <c r="E25" s="3">
+      <c r="I25" s="14">
         <v>0</v>
       </c>
-      <c r="F25" s="3">
-        <v>30</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>25</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>1</v>
@@ -1137,7 +1277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
@@ -1165,32 +1305,32 @@
       <c r="I32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>1</v>
       </c>
@@ -1218,138 +1358,138 @@
       <c r="I33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P35" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1377,138 +1517,147 @@
       <c r="I36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q36" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R36" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q37" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R37" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q38" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1536,37 +1685,384 @@
       <c r="I39" s="3">
         <v>15</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="14">
+        <v>30</v>
+      </c>
+      <c r="K39" s="14">
         <v>25</v>
       </c>
-      <c r="K39" s="3">
+      <c r="L39" s="14">
+        <v>0</v>
+      </c>
+      <c r="M39" s="14">
+        <v>0</v>
+      </c>
+      <c r="N39" s="14">
+        <v>0</v>
+      </c>
+      <c r="O39" s="14">
+        <v>0</v>
+      </c>
+      <c r="P39" s="14">
+        <v>15</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q40" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>5</v>
+      </c>
+      <c r="G44" s="1">
+        <v>6</v>
+      </c>
+      <c r="H44" s="1">
+        <v>7</v>
+      </c>
+      <c r="I44" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="3">
         <v>10</v>
       </c>
-      <c r="L39" s="3">
+      <c r="C52" s="3">
+        <v>10</v>
+      </c>
+      <c r="D52" s="3">
         <v>0</v>
       </c>
-      <c r="M39" s="3">
+      <c r="E52" s="3">
         <v>0</v>
       </c>
-      <c r="N39" s="3">
+      <c r="F52" s="14">
+        <v>25</v>
+      </c>
+      <c r="G52" s="14">
         <v>0</v>
       </c>
-      <c r="O39" s="3">
+      <c r="H52" s="14">
+        <v>15</v>
+      </c>
+      <c r="I52" s="14">
         <v>0</v>
       </c>
-      <c r="P39" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="250" spans="279:300" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="250" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS250" s="1"/>
       <c r="JT250" s="1"/>
       <c r="JU250" s="1"/>
@@ -1590,7 +2086,7 @@
       <c r="KM250" s="1"/>
       <c r="KN250" s="1"/>
     </row>
-    <row r="251" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="251" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS251" s="3"/>
       <c r="JT251" s="3"/>
       <c r="JU251" s="3"/>
@@ -1614,7 +2110,7 @@
       <c r="KM251" s="3"/>
       <c r="KN251" s="3"/>
     </row>
-    <row r="252" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="252" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS252" s="3"/>
       <c r="JT252" s="3"/>
       <c r="JU252" s="3"/>
@@ -1638,7 +2134,7 @@
       <c r="KM252" s="3"/>
       <c r="KN252" s="3"/>
     </row>
-    <row r="253" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="253" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS253" s="3"/>
       <c r="JT253" s="3"/>
       <c r="JU253" s="3"/>
@@ -1662,7 +2158,7 @@
       <c r="KM253" s="3"/>
       <c r="KN253" s="3"/>
     </row>
-    <row r="254" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="254" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS254" s="3"/>
       <c r="JT254" s="3"/>
       <c r="JU254" s="3"/>
@@ -1686,7 +2182,7 @@
       <c r="KM254" s="3"/>
       <c r="KN254" s="3"/>
     </row>
-    <row r="255" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="255" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS255" s="3"/>
       <c r="JT255" s="3"/>
       <c r="JU255" s="3"/>
@@ -1710,7 +2206,7 @@
       <c r="KM255" s="3"/>
       <c r="KN255" s="3"/>
     </row>
-    <row r="256" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="256" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS256" s="3"/>
       <c r="JT256" s="3"/>
       <c r="JU256" s="3"/>
@@ -1734,7 +2230,7 @@
       <c r="KM256" s="3"/>
       <c r="KN256" s="3"/>
     </row>
-    <row r="257" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="257" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS257" s="3"/>
       <c r="JT257" s="3"/>
       <c r="JU257" s="3"/>
@@ -1758,7 +2254,7 @@
       <c r="KM257" s="3"/>
       <c r="KN257" s="3"/>
     </row>
-    <row r="258" spans="279:300" x14ac:dyDescent="0.25">
+    <row r="258" spans="279:300" x14ac:dyDescent="0.2">
       <c r="JS258" s="3"/>
       <c r="JT258" s="3"/>
       <c r="JU258" s="3"/>

</xml_diff>